<commit_message>
ConfigInputs done. ReadInputs generator started.
</commit_message>
<xml_diff>
--- a/Config Files/Inputs_V0.xlsx
+++ b/Config Files/Inputs_V0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C535461-9BB0-40C1-899B-05293C86302A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3D6E2C-4566-45C4-8B60-5DB3057C4D77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="192">
   <si>
     <t>Version: 1</t>
   </si>
@@ -531,9 +531,6 @@
     <t>STATES</t>
   </si>
   <si>
-    <t>CLOSED STATES</t>
-  </si>
-  <si>
     <t>FIRE_DAMPR_CLOSED_EN_ADDR</t>
   </si>
   <si>
@@ -592,6 +589,18 @@
   </si>
   <si>
     <t>NotClosed*Closed*Auto</t>
+  </si>
+  <si>
+    <t>FIRE_DAMPR_DATA_TYPE</t>
+  </si>
+  <si>
+    <t>VAV_SWITCHES_DATA_TYPE</t>
+  </si>
+  <si>
+    <t>CLOSED_STATES</t>
+  </si>
+  <si>
+    <t>ROOM_PRESSURES_DATA_TYPE</t>
   </si>
 </sst>
 </file>
@@ -1716,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U93"/>
+  <dimension ref="A1:U96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1788,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1787,7 +1796,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>802</v>
@@ -1795,10 +1804,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B5">
-        <v>501</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1806,15 +1815,15 @@
         <v>172</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1822,7 +1831,7 @@
         <v>170</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,84 +1839,84 @@
         <v>169</v>
       </c>
       <c r="B9">
-        <v>824</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>187</v>
+        <v>168</v>
+      </c>
+      <c r="B10">
+        <v>824</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B12">
-        <v>830</v>
+      <c r="A12" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1915,10 +1924,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>830</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1926,7 +1935,7 @@
         <v>183</v>
       </c>
       <c r="B15">
-        <v>301</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1934,36 +1943,36 @@
         <v>182</v>
       </c>
       <c r="B16">
-        <v>267</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B17">
+      <c r="B18">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19">
-        <v>811</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1971,18 +1980,18 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B21">
-        <v>201</v>
+        <v>811</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B22">
-        <v>287</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -1990,321 +1999,150 @@
         <v>176</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="28" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>822</v>
-      </c>
-      <c r="F27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>171</v>
-      </c>
-      <c r="K27" t="s">
-        <v>17</v>
-      </c>
-      <c r="L27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>823</v>
-      </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>172</v>
-      </c>
-      <c r="K28" t="s">
-        <v>17</v>
-      </c>
-      <c r="L28" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U28" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>825</v>
-      </c>
-      <c r="F29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>173</v>
-      </c>
-      <c r="K29" t="s">
-        <v>17</v>
-      </c>
-      <c r="L29" t="s">
-        <v>17</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>803</v>
+        <v>822</v>
       </c>
       <c r="F30" t="s">
         <v>17</v>
@@ -2319,7 +2157,7 @@
         <v>1</v>
       </c>
       <c r="J30">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K30" t="s">
         <v>17</v>
@@ -2357,16 +2195,16 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>823</v>
@@ -2374,8 +2212,8 @@
       <c r="F31" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>30</v>
+      <c r="G31" t="s">
+        <v>17</v>
       </c>
       <c r="H31" t="s">
         <v>17</v>
@@ -2384,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="J31">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K31" t="s">
         <v>17</v>
@@ -2393,48 +2231,48 @@
         <v>17</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>806</v>
+        <v>825</v>
       </c>
       <c r="F32" t="s">
         <v>17</v>
@@ -2449,7 +2287,7 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K32" t="s">
         <v>17</v>
@@ -2487,19 +2325,19 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F33" t="s">
         <v>17</v>
@@ -2514,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K33" t="s">
         <v>17</v>
@@ -2523,54 +2361,54 @@
         <v>17</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>808</v>
+        <v>823</v>
       </c>
       <c r="F34" t="s">
         <v>17</v>
       </c>
-      <c r="G34" t="s">
-        <v>17</v>
+      <c r="G34" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="H34" t="s">
         <v>17</v>
@@ -2579,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K34" t="s">
         <v>17</v>
@@ -2588,48 +2426,48 @@
         <v>17</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F35" t="s">
         <v>17</v>
@@ -2644,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K35" t="s">
         <v>17</v>
@@ -2653,48 +2491,48 @@
         <v>17</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>831</v>
+        <v>807</v>
       </c>
       <c r="F36" t="s">
         <v>17</v>
@@ -2706,10 +2544,10 @@
         <v>17</v>
       </c>
       <c r="I36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J36">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="K36" t="s">
         <v>17</v>
@@ -2718,48 +2556,48 @@
         <v>17</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>832</v>
+        <v>808</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -2771,10 +2609,10 @@
         <v>17</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="K37" t="s">
         <v>17</v>
@@ -2783,59 +2621,119 @@
         <v>17</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>14</v>
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>809</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>179</v>
+      </c>
+      <c r="K38" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" t="s">
+        <v>17</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>802</v>
+        <v>831</v>
       </c>
       <c r="F39" t="s">
         <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="H39" t="s">
         <v>17</v>
@@ -2844,57 +2742,57 @@
         <v>3</v>
       </c>
       <c r="J39">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K39" t="s">
-        <v>54</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39" t="s">
-        <v>17</v>
-      </c>
-      <c r="N39" t="s">
-        <v>17</v>
-      </c>
-      <c r="O39" t="s">
-        <v>17</v>
-      </c>
-      <c r="P39" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>17</v>
-      </c>
-      <c r="R39" t="s">
-        <v>17</v>
-      </c>
-      <c r="S39" t="s">
-        <v>17</v>
-      </c>
-      <c r="T39" t="s">
-        <v>17</v>
-      </c>
-      <c r="U39" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="L39" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C40">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F40" t="s">
         <v>17</v>
@@ -2909,128 +2807,68 @@
         <v>3</v>
       </c>
       <c r="J40">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K40" t="s">
-        <v>58</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="M40" t="s">
-        <v>17</v>
-      </c>
-      <c r="N40" t="s">
-        <v>17</v>
-      </c>
-      <c r="O40" t="s">
-        <v>17</v>
-      </c>
-      <c r="P40" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>17</v>
-      </c>
-      <c r="R40" t="s">
-        <v>17</v>
-      </c>
-      <c r="S40" t="s">
-        <v>17</v>
-      </c>
-      <c r="T40" t="s">
-        <v>17</v>
-      </c>
-      <c r="U40" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="L40" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41">
+      <c r="A41" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>834</v>
-      </c>
-      <c r="F41" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" t="s">
-        <v>17</v>
-      </c>
-      <c r="H41" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41">
-        <v>3</v>
-      </c>
-      <c r="J41">
-        <v>42</v>
-      </c>
-      <c r="K41" t="s">
-        <v>58</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="M41" t="s">
-        <v>17</v>
-      </c>
-      <c r="N41" t="s">
-        <v>17</v>
-      </c>
-      <c r="O41" t="s">
-        <v>17</v>
-      </c>
-      <c r="P41" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>17</v>
-      </c>
-      <c r="R41" t="s">
-        <v>17</v>
-      </c>
-      <c r="S41" t="s">
-        <v>17</v>
-      </c>
-      <c r="T41" t="s">
-        <v>17</v>
-      </c>
-      <c r="U41" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C42">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>835</v>
+        <v>802</v>
       </c>
       <c r="F42" t="s">
         <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H42" t="s">
         <v>17</v>
@@ -3039,13 +2877,13 @@
         <v>3</v>
       </c>
       <c r="J42">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" t="s">
         <v>17</v>
@@ -3077,19 +2915,19 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="F43" t="s">
         <v>17</v>
@@ -3104,7 +2942,7 @@
         <v>3</v>
       </c>
       <c r="J43">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K43" t="s">
         <v>58</v>
@@ -3142,19 +2980,19 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C44">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="F44" t="s">
         <v>17</v>
@@ -3169,7 +3007,7 @@
         <v>3</v>
       </c>
       <c r="J44">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K44" t="s">
         <v>58</v>
@@ -3207,19 +3045,19 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C45">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="F45" t="s">
         <v>17</v>
@@ -3234,7 +3072,7 @@
         <v>3</v>
       </c>
       <c r="J45">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K45" t="s">
         <v>58</v>
@@ -3272,19 +3110,19 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C46">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="F46" t="s">
         <v>17</v>
@@ -3299,7 +3137,7 @@
         <v>3</v>
       </c>
       <c r="J46">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K46" t="s">
         <v>58</v>
@@ -3337,19 +3175,19 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="F47" t="s">
         <v>17</v>
@@ -3364,7 +3202,7 @@
         <v>3</v>
       </c>
       <c r="J47">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K47" t="s">
         <v>58</v>
@@ -3402,19 +3240,19 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C48">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="F48" t="s">
         <v>17</v>
@@ -3429,7 +3267,7 @@
         <v>3</v>
       </c>
       <c r="J48">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K48" t="s">
         <v>58</v>
@@ -3467,19 +3305,19 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C49">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="F49" t="s">
         <v>17</v>
@@ -3494,7 +3332,7 @@
         <v>3</v>
       </c>
       <c r="J49">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K49" t="s">
         <v>58</v>
@@ -3532,19 +3370,19 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>117</v>
+        <v>74</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C50">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="F50" t="s">
         <v>17</v>
@@ -3559,7 +3397,7 @@
         <v>3</v>
       </c>
       <c r="J50">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K50" t="s">
         <v>58</v>
@@ -3597,19 +3435,19 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>118</v>
+        <v>75</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C51">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="F51" t="s">
         <v>17</v>
@@ -3624,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="J51">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K51" t="s">
         <v>58</v>
@@ -3662,19 +3500,19 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>119</v>
+        <v>76</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="C52">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="F52" t="s">
         <v>17</v>
@@ -3689,7 +3527,7 @@
         <v>3</v>
       </c>
       <c r="J52">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K52" t="s">
         <v>58</v>
@@ -3727,19 +3565,19 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C53">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="F53" t="s">
         <v>17</v>
@@ -3754,7 +3592,7 @@
         <v>3</v>
       </c>
       <c r="J53">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K53" t="s">
         <v>58</v>
@@ -3792,19 +3630,19 @@
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C54">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="F54" t="s">
         <v>17</v>
@@ -3819,7 +3657,7 @@
         <v>3</v>
       </c>
       <c r="J54">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K54" t="s">
         <v>58</v>
@@ -3857,19 +3695,19 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C55">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F55" t="s">
         <v>17</v>
@@ -3884,7 +3722,7 @@
         <v>3</v>
       </c>
       <c r="J55">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K55" t="s">
         <v>58</v>
@@ -3922,19 +3760,19 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C56">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="F56" t="s">
         <v>17</v>
@@ -3949,7 +3787,7 @@
         <v>3</v>
       </c>
       <c r="J56">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K56" t="s">
         <v>58</v>
@@ -3987,19 +3825,19 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="F57" t="s">
         <v>17</v>
@@ -4014,7 +3852,7 @@
         <v>3</v>
       </c>
       <c r="J57">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K57" t="s">
         <v>58</v>
@@ -4052,19 +3890,19 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C58">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="F58" t="s">
         <v>17</v>
@@ -4079,13 +3917,13 @@
         <v>3</v>
       </c>
       <c r="J58">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K58" t="s">
         <v>58</v>
       </c>
       <c r="L58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58" t="s">
         <v>17</v>
@@ -4117,19 +3955,19 @@
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C59">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="F59" t="s">
         <v>17</v>
@@ -4144,13 +3982,13 @@
         <v>3</v>
       </c>
       <c r="J59">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K59" t="s">
         <v>58</v>
       </c>
       <c r="L59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" t="s">
         <v>17</v>
@@ -4182,19 +4020,19 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C60">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="F60" t="s">
         <v>17</v>
@@ -4209,13 +4047,13 @@
         <v>3</v>
       </c>
       <c r="J60">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K60" t="s">
         <v>58</v>
       </c>
       <c r="L60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" t="s">
         <v>17</v>
@@ -4247,19 +4085,19 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C61">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -4274,7 +4112,7 @@
         <v>3</v>
       </c>
       <c r="J61">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K61" t="s">
         <v>58</v>
@@ -4312,19 +4150,19 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C62">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="F62" t="s">
         <v>17</v>
@@ -4339,7 +4177,7 @@
         <v>3</v>
       </c>
       <c r="J62">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K62" t="s">
         <v>58</v>
@@ -4377,19 +4215,19 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C63">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="F63" t="s">
         <v>17</v>
@@ -4404,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="J63">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K63" t="s">
         <v>58</v>
@@ -4442,19 +4280,19 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C64">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="F64" t="s">
         <v>17</v>
@@ -4469,7 +4307,7 @@
         <v>3</v>
       </c>
       <c r="J64">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K64" t="s">
         <v>58</v>
@@ -4507,19 +4345,19 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C65">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F65" t="s">
         <v>17</v>
@@ -4534,7 +4372,7 @@
         <v>3</v>
       </c>
       <c r="J65">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K65" t="s">
         <v>58</v>
@@ -4572,19 +4410,19 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C66">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F66" t="s">
         <v>17</v>
@@ -4599,7 +4437,7 @@
         <v>3</v>
       </c>
       <c r="J66">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K66" t="s">
         <v>58</v>
@@ -4637,19 +4475,19 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C67">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -4664,7 +4502,7 @@
         <v>3</v>
       </c>
       <c r="J67">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K67" t="s">
         <v>58</v>
@@ -4702,19 +4540,19 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C68">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="F68" t="s">
         <v>17</v>
@@ -4729,10 +4567,10 @@
         <v>3</v>
       </c>
       <c r="J68">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K68" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L68">
         <v>0</v>
@@ -4767,19 +4605,19 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C69">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F69" t="s">
         <v>17</v>
@@ -4794,10 +4632,10 @@
         <v>3</v>
       </c>
       <c r="J69">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K69" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L69">
         <v>0</v>
@@ -4832,19 +4670,19 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C70">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -4859,10 +4697,10 @@
         <v>3</v>
       </c>
       <c r="J70">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K70" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L70">
         <v>0</v>
@@ -4897,19 +4735,19 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C71">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -4924,7 +4762,7 @@
         <v>3</v>
       </c>
       <c r="J71">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K71" t="s">
         <v>54</v>
@@ -4962,19 +4800,19 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C72">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="F72" t="s">
         <v>17</v>
@@ -4989,7 +4827,7 @@
         <v>3</v>
       </c>
       <c r="J72">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K72" t="s">
         <v>54</v>
@@ -5027,19 +4865,19 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C73">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -5054,7 +4892,7 @@
         <v>3</v>
       </c>
       <c r="J73">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K73" t="s">
         <v>54</v>
@@ -5092,19 +4930,19 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C74">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -5119,7 +4957,7 @@
         <v>3</v>
       </c>
       <c r="J74">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K74" t="s">
         <v>54</v>
@@ -5157,19 +4995,19 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C75">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
@@ -5184,7 +5022,7 @@
         <v>3</v>
       </c>
       <c r="J75">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K75" t="s">
         <v>54</v>
@@ -5222,19 +5060,19 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C76">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="F76" t="s">
         <v>17</v>
@@ -5249,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="J76">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K76" t="s">
         <v>54</v>
@@ -5287,19 +5125,19 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C77">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="F77" t="s">
         <v>17</v>
@@ -5314,7 +5152,7 @@
         <v>3</v>
       </c>
       <c r="J77">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K77" t="s">
         <v>54</v>
@@ -5352,19 +5190,19 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C78">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="F78" t="s">
         <v>17</v>
@@ -5379,7 +5217,7 @@
         <v>3</v>
       </c>
       <c r="J78">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K78" t="s">
         <v>54</v>
@@ -5417,19 +5255,19 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C79">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -5444,7 +5282,7 @@
         <v>3</v>
       </c>
       <c r="J79">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K79" t="s">
         <v>54</v>
@@ -5482,19 +5320,19 @@
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C80">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="F80" t="s">
         <v>17</v>
@@ -5509,7 +5347,7 @@
         <v>3</v>
       </c>
       <c r="J80">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K80" t="s">
         <v>54</v>
@@ -5547,19 +5385,19 @@
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C81">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="F81" t="s">
         <v>17</v>
@@ -5574,7 +5412,7 @@
         <v>3</v>
       </c>
       <c r="J81">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K81" t="s">
         <v>54</v>
@@ -5612,19 +5450,19 @@
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C82">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="F82" t="s">
         <v>17</v>
@@ -5639,7 +5477,7 @@
         <v>3</v>
       </c>
       <c r="J82">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K82" t="s">
         <v>54</v>
@@ -5677,19 +5515,19 @@
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C83">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="F83" t="s">
         <v>17</v>
@@ -5704,7 +5542,7 @@
         <v>3</v>
       </c>
       <c r="J83">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K83" t="s">
         <v>54</v>
@@ -5742,19 +5580,19 @@
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C84">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="F84" t="s">
         <v>17</v>
@@ -5769,7 +5607,7 @@
         <v>3</v>
       </c>
       <c r="J84">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K84" t="s">
         <v>54</v>
@@ -5807,19 +5645,19 @@
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C85">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="F85" t="s">
         <v>17</v>
@@ -5834,7 +5672,7 @@
         <v>3</v>
       </c>
       <c r="J85">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K85" t="s">
         <v>54</v>
@@ -5872,19 +5710,19 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C86">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="F86" t="s">
         <v>17</v>
@@ -5899,7 +5737,7 @@
         <v>3</v>
       </c>
       <c r="J86">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K86" t="s">
         <v>54</v>
@@ -5937,19 +5775,19 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C87">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="F87" t="s">
         <v>17</v>
@@ -5964,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="J87">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K87" t="s">
         <v>54</v>
@@ -6002,19 +5840,19 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C88">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="F88" t="s">
         <v>17</v>
@@ -6029,13 +5867,13 @@
         <v>3</v>
       </c>
       <c r="J88">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K88" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M88" t="s">
         <v>17</v>
@@ -6067,19 +5905,19 @@
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C89">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="F89" t="s">
         <v>17</v>
@@ -6094,13 +5932,13 @@
         <v>3</v>
       </c>
       <c r="J89">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K89" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M89" t="s">
         <v>17</v>
@@ -6132,34 +5970,34 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C90">
-        <v>63</v>
-      </c>
-      <c r="D90" t="s">
-        <v>17</v>
-      </c>
-      <c r="E90" t="s">
-        <v>17</v>
-      </c>
-      <c r="F90">
-        <v>2</v>
+        <v>60</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>874</v>
+      </c>
+      <c r="F90" t="s">
+        <v>17</v>
       </c>
       <c r="G90" t="s">
         <v>17</v>
       </c>
-      <c r="H90">
-        <v>23</v>
+      <c r="H90" t="s">
+        <v>17</v>
       </c>
       <c r="I90">
         <v>3</v>
       </c>
       <c r="J90">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="K90" t="s">
         <v>54</v>
@@ -6197,40 +6035,40 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C91">
-        <v>64</v>
-      </c>
-      <c r="D91" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" t="s">
-        <v>17</v>
-      </c>
-      <c r="F91">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>875</v>
+      </c>
+      <c r="F91" t="s">
+        <v>17</v>
       </c>
       <c r="G91" t="s">
         <v>17</v>
       </c>
-      <c r="H91">
-        <v>23</v>
+      <c r="H91" t="s">
+        <v>17</v>
       </c>
       <c r="I91">
         <v>3</v>
       </c>
       <c r="J91">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="K91" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="L91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M91" t="s">
         <v>17</v>
@@ -6262,40 +6100,40 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C92">
-        <v>65</v>
-      </c>
-      <c r="D92" t="s">
-        <v>17</v>
-      </c>
-      <c r="E92" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>876</v>
+      </c>
+      <c r="F92" t="s">
+        <v>17</v>
       </c>
       <c r="G92" t="s">
         <v>17</v>
       </c>
-      <c r="H92">
-        <v>24</v>
+      <c r="H92" t="s">
+        <v>17</v>
       </c>
       <c r="I92">
         <v>3</v>
       </c>
       <c r="J92">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="K92" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M92" t="s">
         <v>17</v>
@@ -6327,13 +6165,13 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C93">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D93" t="s">
         <v>17</v>
@@ -6348,16 +6186,16 @@
         <v>17</v>
       </c>
       <c r="H93">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I93">
         <v>3</v>
       </c>
       <c r="J93">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="K93" t="s">
-        <v>163</v>
+        <v>54</v>
       </c>
       <c r="L93">
         <v>0</v>
@@ -6390,528 +6228,723 @@
         <v>17</v>
       </c>
     </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94">
+        <v>64</v>
+      </c>
+      <c r="D94" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" t="s">
+        <v>17</v>
+      </c>
+      <c r="F94">
+        <v>2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94">
+        <v>23</v>
+      </c>
+      <c r="I94">
+        <v>3</v>
+      </c>
+      <c r="J94">
+        <v>132</v>
+      </c>
+      <c r="K94" t="s">
+        <v>163</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94" t="s">
+        <v>17</v>
+      </c>
+      <c r="N94" t="s">
+        <v>17</v>
+      </c>
+      <c r="O94" t="s">
+        <v>17</v>
+      </c>
+      <c r="P94" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>17</v>
+      </c>
+      <c r="R94" t="s">
+        <v>17</v>
+      </c>
+      <c r="S94" t="s">
+        <v>17</v>
+      </c>
+      <c r="T94" t="s">
+        <v>17</v>
+      </c>
+      <c r="U94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C95">
+        <v>65</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" t="s">
+        <v>17</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95">
+        <v>24</v>
+      </c>
+      <c r="I95">
+        <v>3</v>
+      </c>
+      <c r="J95">
+        <v>146</v>
+      </c>
+      <c r="K95" t="s">
+        <v>54</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95" t="s">
+        <v>17</v>
+      </c>
+      <c r="N95" t="s">
+        <v>17</v>
+      </c>
+      <c r="O95" t="s">
+        <v>17</v>
+      </c>
+      <c r="P95" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>17</v>
+      </c>
+      <c r="R95" t="s">
+        <v>17</v>
+      </c>
+      <c r="S95" t="s">
+        <v>17</v>
+      </c>
+      <c r="T95" t="s">
+        <v>17</v>
+      </c>
+      <c r="U95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C96">
+        <v>66</v>
+      </c>
+      <c r="D96" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" t="s">
+        <v>17</v>
+      </c>
+      <c r="F96">
+        <v>2</v>
+      </c>
+      <c r="G96" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96">
+        <v>24</v>
+      </c>
+      <c r="I96">
+        <v>3</v>
+      </c>
+      <c r="J96">
+        <v>147</v>
+      </c>
+      <c r="K96" t="s">
+        <v>163</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96" t="s">
+        <v>17</v>
+      </c>
+      <c r="N96" t="s">
+        <v>17</v>
+      </c>
+      <c r="O96" t="s">
+        <v>17</v>
+      </c>
+      <c r="P96" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>17</v>
+      </c>
+      <c r="R96" t="s">
+        <v>17</v>
+      </c>
+      <c r="S96" t="s">
+        <v>17</v>
+      </c>
+      <c r="T96" t="s">
+        <v>17</v>
+      </c>
+      <c r="U96" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A27">
+  <conditionalFormatting sqref="A30">
     <cfRule type="cellIs" dxfId="104" priority="105" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
+  <conditionalFormatting sqref="A30">
     <cfRule type="cellIs" dxfId="103" priority="104" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
+  <conditionalFormatting sqref="A31">
     <cfRule type="cellIs" dxfId="102" priority="103" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
+  <conditionalFormatting sqref="A31">
     <cfRule type="cellIs" dxfId="101" priority="102" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
+  <conditionalFormatting sqref="A32">
     <cfRule type="cellIs" dxfId="100" priority="101" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
+  <conditionalFormatting sqref="A32">
     <cfRule type="cellIs" dxfId="99" priority="100" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
+  <conditionalFormatting sqref="A33">
     <cfRule type="cellIs" dxfId="98" priority="99" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
+  <conditionalFormatting sqref="A33">
     <cfRule type="cellIs" dxfId="97" priority="98" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
+  <conditionalFormatting sqref="B33">
     <cfRule type="cellIs" dxfId="96" priority="97" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
+  <conditionalFormatting sqref="B33">
     <cfRule type="cellIs" dxfId="95" priority="96" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
+  <conditionalFormatting sqref="A34">
     <cfRule type="cellIs" dxfId="94" priority="95" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
+  <conditionalFormatting sqref="A34">
     <cfRule type="cellIs" dxfId="93" priority="94" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+  <conditionalFormatting sqref="A35">
     <cfRule type="cellIs" dxfId="92" priority="93" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+  <conditionalFormatting sqref="A35">
     <cfRule type="cellIs" dxfId="91" priority="92" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
+  <conditionalFormatting sqref="A36">
     <cfRule type="cellIs" dxfId="90" priority="91" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
+  <conditionalFormatting sqref="A36">
     <cfRule type="cellIs" dxfId="89" priority="90" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+  <conditionalFormatting sqref="A37">
     <cfRule type="cellIs" dxfId="88" priority="89" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+  <conditionalFormatting sqref="A37">
     <cfRule type="cellIs" dxfId="87" priority="88" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+  <conditionalFormatting sqref="A38">
     <cfRule type="cellIs" dxfId="86" priority="87" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+  <conditionalFormatting sqref="A38">
     <cfRule type="cellIs" dxfId="85" priority="86" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A39">
     <cfRule type="cellIs" dxfId="84" priority="85" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A39">
     <cfRule type="cellIs" dxfId="83" priority="84" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A40">
     <cfRule type="cellIs" dxfId="82" priority="83" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A40">
     <cfRule type="cellIs" dxfId="81" priority="82" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M36:U37">
+  <conditionalFormatting sqref="M39:U40">
     <cfRule type="cellIs" dxfId="80" priority="81" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M36:U37">
+  <conditionalFormatting sqref="M39:U40">
     <cfRule type="cellIs" dxfId="79" priority="80" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M40:U40">
+    <cfRule type="cellIs" dxfId="78" priority="79" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M40:U40">
+    <cfRule type="cellIs" dxfId="77" priority="78" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M39:U39">
+    <cfRule type="cellIs" dxfId="76" priority="77" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M39:U39">
+    <cfRule type="cellIs" dxfId="75" priority="76" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38:U38">
+    <cfRule type="cellIs" dxfId="74" priority="75" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38:U38">
+    <cfRule type="cellIs" dxfId="73" priority="74" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38:U38">
+    <cfRule type="cellIs" dxfId="72" priority="72" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38:U38">
+    <cfRule type="cellIs" dxfId="71" priority="73" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M37:U37">
-    <cfRule type="cellIs" dxfId="78" priority="79" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="71" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M37:U37">
-    <cfRule type="cellIs" dxfId="77" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M37:U37">
+    <cfRule type="cellIs" dxfId="68" priority="68" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M37:U37">
+    <cfRule type="cellIs" dxfId="67" priority="69" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30:U30 M34:U36">
+    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30:U30 M34:U36">
+    <cfRule type="cellIs" dxfId="65" priority="66" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34:U34">
+    <cfRule type="cellIs" dxfId="64" priority="65" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M36:U36">
-    <cfRule type="cellIs" dxfId="76" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M36:U36">
-    <cfRule type="cellIs" dxfId="75" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35:U35">
-    <cfRule type="cellIs" dxfId="74" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35:U35">
-    <cfRule type="cellIs" dxfId="73" priority="74" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M35:U35">
-    <cfRule type="cellIs" dxfId="72" priority="72" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M35:U35">
-    <cfRule type="cellIs" dxfId="71" priority="73" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:U34">
-    <cfRule type="cellIs" dxfId="70" priority="71" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:U34">
-    <cfRule type="cellIs" dxfId="69" priority="70" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:U34">
-    <cfRule type="cellIs" dxfId="68" priority="68" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:U34">
-    <cfRule type="cellIs" dxfId="67" priority="69" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M27:U27 M31:U33">
-    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M27:U27 M31:U33">
-    <cfRule type="cellIs" dxfId="65" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="61" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:U33">
+    <cfRule type="cellIs" dxfId="59" priority="60" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:U33">
+    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M33:U33">
+    <cfRule type="cellIs" dxfId="57" priority="58" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M33:U33">
+    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:U32">
+    <cfRule type="cellIs" dxfId="55" priority="56" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:U32">
+    <cfRule type="cellIs" dxfId="54" priority="55" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30:U30">
+    <cfRule type="cellIs" dxfId="53" priority="54" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30:U30">
+    <cfRule type="cellIs" dxfId="52" priority="53" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:U31">
-    <cfRule type="cellIs" dxfId="64" priority="65" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M33:U33">
-    <cfRule type="cellIs" dxfId="63" priority="63" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M33:U33">
-    <cfRule type="cellIs" dxfId="62" priority="64" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M32:U32">
-    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M32:U32">
-    <cfRule type="cellIs" dxfId="60" priority="61" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29:U30">
-    <cfRule type="cellIs" dxfId="59" priority="60" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29:U30">
-    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M30:U30">
-    <cfRule type="cellIs" dxfId="57" priority="58" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M30:U30">
-    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29:U29">
-    <cfRule type="cellIs" dxfId="55" priority="56" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29:U29">
-    <cfRule type="cellIs" dxfId="54" priority="55" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M27:U27">
-    <cfRule type="cellIs" dxfId="53" priority="54" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M27:U27">
-    <cfRule type="cellIs" dxfId="52" priority="53" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M28:U28">
     <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:U28">
+  <conditionalFormatting sqref="M31:U31">
     <cfRule type="cellIs" dxfId="50" priority="51" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:U28">
+  <conditionalFormatting sqref="M31:U31">
     <cfRule type="cellIs" dxfId="49" priority="50" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:U28">
+  <conditionalFormatting sqref="M31:U31">
     <cfRule type="cellIs" dxfId="48" priority="49" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+  <conditionalFormatting sqref="A42">
     <cfRule type="cellIs" dxfId="47" priority="48" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+  <conditionalFormatting sqref="A42">
     <cfRule type="cellIs" dxfId="46" priority="47" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
+  <conditionalFormatting sqref="A43">
     <cfRule type="cellIs" dxfId="45" priority="46" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
+  <conditionalFormatting sqref="A43">
     <cfRule type="cellIs" dxfId="44" priority="45" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
+  <conditionalFormatting sqref="A44">
     <cfRule type="cellIs" dxfId="43" priority="44" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
+  <conditionalFormatting sqref="A44">
     <cfRule type="cellIs" dxfId="42" priority="43" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+  <conditionalFormatting sqref="A45">
     <cfRule type="cellIs" dxfId="41" priority="42" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+  <conditionalFormatting sqref="A45">
     <cfRule type="cellIs" dxfId="40" priority="41" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
+  <conditionalFormatting sqref="A46">
     <cfRule type="cellIs" dxfId="39" priority="40" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
+  <conditionalFormatting sqref="A46">
     <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
+  <conditionalFormatting sqref="A47">
     <cfRule type="cellIs" dxfId="37" priority="38" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
+  <conditionalFormatting sqref="A47">
     <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
+  <conditionalFormatting sqref="A48">
     <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
+  <conditionalFormatting sqref="A48">
     <cfRule type="cellIs" dxfId="34" priority="35" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A46:A49">
+  <conditionalFormatting sqref="A49:A52">
     <cfRule type="cellIs" dxfId="33" priority="34" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A46:A49">
+  <conditionalFormatting sqref="A49:A52">
     <cfRule type="cellIs" dxfId="32" priority="33" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:A73 A84:A89">
+  <conditionalFormatting sqref="A53:A76 A87:A92">
     <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:A73 A84:A89">
+  <conditionalFormatting sqref="A53:A76 A87:A92">
     <cfRule type="cellIs" dxfId="30" priority="31" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A83">
+  <conditionalFormatting sqref="A77:A86">
     <cfRule type="cellIs" dxfId="29" priority="30" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A83">
+  <conditionalFormatting sqref="A77:A86">
     <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:B61 B68:B89">
+  <conditionalFormatting sqref="B53:B64 B71:B92">
     <cfRule type="cellIs" dxfId="27" priority="28" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:B61 B68:B89">
+  <conditionalFormatting sqref="B53:B64 B71:B92">
     <cfRule type="cellIs" dxfId="26" priority="27" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B67">
+  <conditionalFormatting sqref="B65:B70">
     <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B67">
+  <conditionalFormatting sqref="B65:B70">
     <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
+  <conditionalFormatting sqref="B80">
     <cfRule type="cellIs" dxfId="23" priority="24" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
+  <conditionalFormatting sqref="B80">
     <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
+  <conditionalFormatting sqref="B64">
     <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
+  <conditionalFormatting sqref="B64">
     <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+  <conditionalFormatting sqref="B62">
     <cfRule type="cellIs" dxfId="19" priority="20" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+  <conditionalFormatting sqref="B62">
     <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90:A93">
+  <conditionalFormatting sqref="A93:A96">
     <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90:A93">
+  <conditionalFormatting sqref="A93:A96">
     <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:B93">
+  <conditionalFormatting sqref="B93:B96">
     <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:B93">
+  <conditionalFormatting sqref="B93:B96">
     <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:K11">
+  <conditionalFormatting sqref="C11:K12">
     <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:K11">
+  <conditionalFormatting sqref="C11:K12">
     <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:K12">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:K11">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:K10">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"To translate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:K10">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:K24">
+  <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:K24">
+  <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:K24">
+  <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:K24">
+  <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"To translate"</formula>
     </cfRule>

</xml_diff>

<commit_message>
more macro options, ReadOutputs almost done
</commit_message>
<xml_diff>
--- a/Config Files/Inputs_V0.xlsx
+++ b/Config Files/Inputs_V0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3D6E2C-4566-45C4-8B60-5DB3057C4D77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E039D8D2-E743-4A0F-83E4-868925CF40A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1728,30 +1728,30 @@
   <dimension ref="A1:U96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="21" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>165</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>174</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>173</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>171</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>172</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>188</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>170</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>169</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>168</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>167</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>190</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>184</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>185</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>183</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>182</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>191</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>181</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>180</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>179</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>178</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>177</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>176</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>189</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>164</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>175</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>167</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -2123,12 +2123,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2843,12 +2843,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>60</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>62</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>68</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>73</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>74</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>75</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>76</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>77</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>78</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>79</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>80</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>81</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>82</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>83</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>84</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>85</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>86</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>87</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>88</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>89</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>90</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>91</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>92</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>93</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>94</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>98</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>99</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>100</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>101</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>102</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>105</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>106</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>107</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>108</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>109</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>110</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>111</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>112</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>113</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>114</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>115</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>116</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>155</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>156</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>157</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>158</v>
       </c>

</xml_diff>